<commit_message>
adding some features to filter in letter search
</commit_message>
<xml_diff>
--- a/Gantt project planner.xlsx
+++ b/Gantt project planner.xlsx
@@ -589,6 +589,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="fill" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -598,6 +610,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -630,24 +648,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="fill" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="fill" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="fill" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1061,20 +1061,20 @@
   <dimension ref="B1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="15.625" style="20" customWidth="1"/>
     <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.625" style="3" customWidth="1"/>
     <col min="8" max="27" width="2.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="22" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="11"/>
@@ -1084,13 +1084,13 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="4" t="s">
         <v>24</v>
       </c>
@@ -1098,66 +1098,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="27"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="27"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="19" t="s">
+      <c r="V2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="29"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="35"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="30" t="s">
+      <c r="AA2" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="38"/>
       <c r="AH2" s="17"/>
-      <c r="AI2" s="19" t="s">
+      <c r="AI2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
+      <c r="AJ2" s="24"/>
+      <c r="AK2" s="24"/>
+      <c r="AL2" s="24"/>
+      <c r="AM2" s="24"/>
+      <c r="AN2" s="24"/>
+      <c r="AO2" s="24"/>
+      <c r="AP2" s="24"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="30" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1184,12 +1184,12 @@
       <c r="AA3" s="9"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="2">
         <v>1</v>
       </c>
@@ -1372,7 +1372,7 @@
       </c>
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="5">
@@ -1382,17 +1382,17 @@
         <v>1</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="5">
@@ -1402,17 +1402,17 @@
         <v>1</v>
       </c>
       <c r="E6" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="5">
@@ -1432,7 +1432,7 @@
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="5">
@@ -1452,7 +1452,7 @@
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="21" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="5">
@@ -1472,7 +1472,7 @@
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="21" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="5">
@@ -1492,7 +1492,7 @@
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="5">
@@ -1512,7 +1512,7 @@
       </c>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="5">
@@ -1532,7 +1532,7 @@
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="5">
@@ -1552,7 +1552,7 @@
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="19" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="5">
@@ -1572,7 +1572,7 @@
       </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="7">
@@ -1592,7 +1592,7 @@
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="5">
@@ -1612,7 +1612,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="5">
@@ -1632,7 +1632,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="5">
@@ -1652,7 +1652,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="5">
@@ -1672,7 +1672,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="5">
@@ -1692,7 +1692,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="5">
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="5">
@@ -1732,7 +1732,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="5">
@@ -1752,7 +1752,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="5">
@@ -1772,7 +1772,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="5">
@@ -1792,7 +1792,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="5">
@@ -1812,7 +1812,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="19" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="5">
@@ -1832,7 +1832,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="5">
@@ -1852,7 +1852,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="5">
@@ -1872,7 +1872,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C30" s="5">

</xml_diff>